<commit_message>
chenged some registers of inverter
</commit_message>
<xml_diff>
--- a/chanales.xlsx
+++ b/chanales.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\projects\gypsum-hmi\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CC7C64-C2D8-4BBF-85AA-0AEBEA6891BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="1968" windowWidth="12480" windowHeight="6828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10560" yWindow="1965" windowWidth="12480" windowHeight="6825"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>konveyr</t>
   </si>
@@ -76,13 +70,37 @@
   </si>
   <si>
     <t>VIBR</t>
+  </si>
+  <si>
+    <t>MILL_AUTO_1-0 bit</t>
+  </si>
+  <si>
+    <t>MILL_AUTO_1-1 bit</t>
+  </si>
+  <si>
+    <t>MILL_AUTO_1-2 bit</t>
+  </si>
+  <si>
+    <t>MILL_AUTO_1-3 bit</t>
+  </si>
+  <si>
+    <t>ESTOP</t>
+  </si>
+  <si>
+    <t>btnSTART</t>
+  </si>
+  <si>
+    <t>btnRESET</t>
+  </si>
+  <si>
+    <t>btnSTOP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +161,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -183,6 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -243,7 +268,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -278,7 +303,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -455,25 +480,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E19" sqref="E18:E19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -481,25 +508,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,25 +534,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
@@ -533,31 +560,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -565,25 +592,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
@@ -591,13 +618,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" s="7" t="s">
         <v>13</v>
       </c>
@@ -605,7 +632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21" s="5" t="s">
         <v>14</v>
       </c>
@@ -613,7 +640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" s="6" t="s">
         <v>9</v>
       </c>
@@ -621,7 +648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23" s="6" t="s">
         <v>10</v>
       </c>
@@ -629,7 +656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24" s="6" t="s">
         <v>15</v>
       </c>
@@ -637,12 +664,44 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>